<commit_message>
QvsNN : zweiter Test
</commit_message>
<xml_diff>
--- a/Sicherung/Test Q vs NN.xlsx
+++ b/Sicherung/Test Q vs NN.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lena\Documents\BAP\Sicherung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lena\Documents\Connect4Console\Sicherung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18514" windowHeight="8554"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18510" windowHeight="8550"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Gewonnen Q-Player</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>Turnier jeweils mit 10.000 Spielen, Q-Player beginnt</t>
+  </si>
+  <si>
+    <t>ein zweiter versuch mit 128er-Datenbank für Q-Player</t>
+  </si>
+  <si>
+    <t>Mittelwerte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in %: </t>
+  </si>
+  <si>
+    <t>Verbesserung der Q-Player in %:</t>
   </si>
 </sst>
 </file>
@@ -63,15 +75,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -94,16 +130,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -418,232 +478,506 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E18"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" customWidth="1"/>
-    <col min="2" max="2" width="13.921875" customWidth="1"/>
-    <col min="5" max="5" width="12.53515625" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="F3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
         <v>7628</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>2371</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>24169</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>7555</v>
+      </c>
+      <c r="H6" s="9">
+        <v>2444</v>
+      </c>
+      <c r="I6" s="9">
+        <v>24150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
         <v>7585</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>2414</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>48595</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9">
+        <v>7590</v>
+      </c>
+      <c r="H7" s="9">
+        <v>2409</v>
+      </c>
+      <c r="I7" s="9">
+        <v>48318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
         <v>7634</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>2366</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>72711</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F8" s="9">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>7630</v>
+      </c>
+      <c r="H8" s="9">
+        <v>2368</v>
+      </c>
+      <c r="I8" s="9">
+        <v>72517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>4</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
         <v>7657</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>2342</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>96761</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>7629</v>
+      </c>
+      <c r="H9" s="9">
+        <v>2371</v>
+      </c>
+      <c r="I9" s="9">
+        <v>96480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>7625</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>2372</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>120862</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>7571</v>
+      </c>
+      <c r="H10" s="9">
+        <v>2429</v>
+      </c>
+      <c r="I10" s="9">
+        <v>120678</v>
+      </c>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="11">
+        <f>AVERAGE(C6:C10)</f>
+        <v>7625.8</v>
+      </c>
+      <c r="D11" s="11">
+        <f>AVERAGE(D6:D10)</f>
+        <v>2373</v>
+      </c>
+      <c r="E11" s="11">
+        <f>AVERAGE(E6:E10)</f>
+        <v>72619.600000000006</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7">
+        <f>AVERAGE(G6:G10)</f>
+        <v>7595</v>
+      </c>
+      <c r="H11" s="7">
+        <f>AVERAGE(H6:H10)</f>
+        <v>2404.1999999999998</v>
+      </c>
+      <c r="I11" s="7">
+        <f>AVERAGE(I6:I10)</f>
+        <v>72428.600000000006</v>
+      </c>
+      <c r="K11">
+        <f>H12-D12</f>
+        <v>0.31199999999999761</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="11">
+        <f>C11/100</f>
+        <v>76.257999999999996</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" ref="D12:I12" si="0">D11/100</f>
+        <v>23.73</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>75.95</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>24.041999999999998</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="0"/>
+        <v>724.28600000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
         <v>7222</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>2778</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>24017</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>7203</v>
+      </c>
+      <c r="H14" s="9">
+        <v>2797</v>
+      </c>
+      <c r="I14" s="9">
+        <v>12036</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
         <v>7256</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>2744</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>35989</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>7232</v>
+      </c>
+      <c r="H15" s="9">
+        <v>2768</v>
+      </c>
+      <c r="I15" s="9">
+        <v>24101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
         <v>7244</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>2756</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>48034</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <v>7207</v>
+      </c>
+      <c r="H16" s="9">
+        <v>2793</v>
+      </c>
+      <c r="I16" s="9">
+        <v>48034</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>4</v>
       </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
         <v>7209</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>2791</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>60003</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>7210</v>
+      </c>
+      <c r="H17" s="9">
+        <v>2790</v>
+      </c>
+      <c r="I17" s="9">
+        <v>48193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>5</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
         <v>7188</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>2812</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>11980</v>
       </c>
+      <c r="F18" s="9">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <v>7231</v>
+      </c>
+      <c r="H18" s="9">
+        <v>2769</v>
+      </c>
+      <c r="I18" s="9">
+        <v>60141</v>
+      </c>
+      <c r="K18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+      <c r="C19" s="11">
+        <f>AVERAGE(C14:C18)</f>
+        <v>7223.8</v>
+      </c>
+      <c r="D19" s="11">
+        <f>AVERAGE(D14:D18)</f>
+        <v>2776.2</v>
+      </c>
+      <c r="E19" s="11">
+        <f>AVERAGE(E14:E18)</f>
+        <v>36004.6</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7">
+        <f>AVERAGE(G14:G18)</f>
+        <v>7216.6</v>
+      </c>
+      <c r="H19" s="7">
+        <f>AVERAGE(H14:H18)</f>
+        <v>2783.4</v>
+      </c>
+      <c r="I19" s="7">
+        <f>AVERAGE(I14:I18)</f>
+        <v>38501</v>
+      </c>
+      <c r="K19">
+        <f>H20-D20</f>
+        <v>7.2000000000002728E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B20" s="5"/>
+      <c r="C20" s="11">
+        <f>C19/100</f>
+        <v>72.238</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" ref="D20:H20" si="1">D19/100</f>
+        <v>27.761999999999997</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7">
+        <f t="shared" si="1"/>
+        <v>72.165999999999997</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="1"/>
+        <v>27.834</v>
+      </c>
+      <c r="I20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>